<commit_message>
[fix] 修复对容器类型的element type为external type时，生成的cs代码错误对external type调用?.Resove的bug
</commit_message>
<xml_diff>
--- a/DesignerConfigs/Datas/test/external_type.xlsx
+++ b/DesignerConfigs/Datas/test/external_type.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\luban_examples\DesignerConfigs\Datas\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\luban_workspace\luban_examples\DesignerConfigs\Datas\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DBA111C5-7BEA-4CB8-943A-31D5D4DFD779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6FED13-72B1-4B2C-A664-44A79B5F019D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30465" yWindow="3255" windowWidth="25335" windowHeight="12915" xr2:uid="{E492294D-1212-4FD5-8923-12DAE04005DA}"/>
+    <workbookView xWindow="4668" yWindow="5232" windowWidth="23040" windowHeight="6144" xr2:uid="{E492294D-1212-4FD5-8923-12DAE04005DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>##</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -63,6 +63,41 @@
   </si>
   <si>
     <t>AIFF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>##type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AudioType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Color</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>list,AudioType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>list,Color</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AIFF</t>
+  </si>
+  <si>
+    <t>audio_types</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>colors</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -87,12 +122,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -109,9 +156,18 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -427,18 +483,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{553EE69E-CCCE-4ABB-B6BB-D32765D3476F}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.875" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" customWidth="1"/>
+    <col min="7" max="7" width="4.44140625" customWidth="1"/>
+    <col min="8" max="8" width="5.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,30 +511,91 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="H2:J2"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>